<commit_message>
Luban Example - Localization auto update
</commit_message>
<xml_diff>
--- a/samples/LubanExample/Data/Data/__enums__.xlsx
+++ b/samples/LubanExample/Data/Data/__enums__.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22536" windowHeight="11231"/>
+    <workbookView windowWidth="17880" windowHeight="9347" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="示例" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
   <si>
     <t>##var</t>
   </si>
@@ -215,6 +215,24 @@
   </si>
   <si>
     <t>EItemType</t>
+  </si>
+  <si>
+    <t>EEquipmentType</t>
+  </si>
+  <si>
+    <t>装备类型</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>防具</t>
+  </si>
+  <si>
+    <t>Jewelry</t>
+  </si>
+  <si>
+    <t>饰品</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1200,7 @@
   <sheetPr/>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1656,8 +1674,8 @@
   <sheetPr/>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -1793,14 +1811,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="7:7">
+    <row r="6" spans="2:9">
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
       <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="7:7">
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="7:9">
       <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="7:7">
+      <c r="H7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="7:9">
       <c r="G8" s="4"/>
+      <c r="H8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="7:7">
       <c r="G9" s="4"/>

</xml_diff>